<commit_message>
before big change to observe
</commit_message>
<xml_diff>
--- a/data/stressor-response_fixed_ARTR.xlsx
+++ b/data/stressor-response_fixed_ARTR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A55D52B-A928-4781-B74E-FFC409F02225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01BE8E-87C0-4396-B7FB-A276BD69BF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2820" yWindow="12492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -15043,7 +15043,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17627,7 +17627,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18500,7 +18500,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18862,7 +18862,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Demo for Marc P
</commit_message>
<xml_diff>
--- a/data/stressor-response_fixed_ARTR.xlsx
+++ b/data/stressor-response_fixed_ARTR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01BE8E-87C0-4396-B7FB-A276BD69BF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902F6CB4-2514-42BE-A522-E38820BEC223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2820" yWindow="12492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -15043,7 +15043,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15084,35 +15084,38 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -15127,15 +15130,18 @@
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -15147,41 +15153,44 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -15201,10 +15210,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
@@ -15216,7 +15225,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>35</v>
@@ -15224,10 +15233,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
@@ -15247,16 +15256,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
@@ -15270,16 +15279,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
@@ -15293,10 +15302,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -15316,16 +15325,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
@@ -15339,59 +15348,56 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
@@ -15406,36 +15412,30 @@
         <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>